<commit_message>
Possibilité de comparaison 2 cycles
</commit_message>
<xml_diff>
--- a/Propriétés air.xlsx
+++ b/Propriétés air.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\quent\Desktop\Projet Siemens\Python entrainement\Turbine\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05B7F001-50E1-4108-8426-7E3FF236A8E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86CC89A4-CC0B-4D8E-ACE2-A9DC7FEFBF15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{FB7A3C27-D8F8-4950-96C5-C0A83EC977C9}"/>
   </bookViews>
@@ -1220,7 +1220,8 @@
   <dimension ref="A1:I36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K29" sqref="K29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>